<commit_message>
Regression excel file done excellent
</commit_message>
<xml_diff>
--- a/7_MATHS/2_Matrix/2_Multiple_Regression.xlsx
+++ b/7_MATHS/2_Matrix/2_Multiple_Regression.xlsx
@@ -8,13 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CourseraPlus\7_MATHS\2_Matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C0A908-8F2B-4A13-AC2E-7A2632410B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7A963D-1839-4732-BFFE-C7F6DB650E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Multi-reg" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="X">'Multi-reg'!$B$4:$F$22</definedName>
+    <definedName name="Xt">'Multi-reg'!$C$27:$U$31</definedName>
+    <definedName name="XtX">'Multi-reg'!$C$34:$G$38</definedName>
+    <definedName name="XtXInv">'Multi-reg'!$C$41:$G$45</definedName>
+    <definedName name="XtY">'Multi-reg'!$J$34:$J$38</definedName>
+    <definedName name="y">'Multi-reg'!$G$4:$G$22</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,8 +43,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Age</t>
   </si>
@@ -61,12 +91,227 @@
   <si>
     <t>(i.e., AGE, SEVERITY, SURGE-MED and ANXIETY) with outputs (i.e, Satisfaction)</t>
   </si>
+  <si>
+    <r>
+      <t>Where X' = X</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>T</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> X= </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>(X</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> X)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">y =  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>β = (X</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> X)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> X</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">y =  </t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="171" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,13 +332,76 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -120,10 +428,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -140,8 +449,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="2" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -161,13 +486,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>95251</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>263660</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>114301</xdr:rowOff>
@@ -222,13 +547,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>161926</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>92629</xdr:rowOff>
@@ -283,13 +608,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>308018</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>560645</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
@@ -324,6 +649,67 @@
         <a:xfrm>
           <a:off x="8870993" y="1076325"/>
           <a:ext cx="3300627" cy="2438400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBC2AA34-2FD9-7EED-0138-977262CF3F5D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6172200" y="3171825"/>
+          <a:ext cx="2457450" cy="771525"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -608,47 +994,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Q22"/>
+  <dimension ref="B2:U45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" style="1" customWidth="1"/>
-    <col min="2" max="6" width="15.85546875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="2" width="3.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:17" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="2:18" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>1</v>
-      </c>
       <c r="D3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -657,328 +1046,914 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R3" s="1"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
         <v>55</v>
       </c>
-      <c r="C4" s="3">
+      <c r="D4" s="3">
         <v>49</v>
       </c>
-      <c r="D4" s="3">
+      <c r="E4" s="3">
         <v>0</v>
       </c>
-      <c r="E4" s="3">
+      <c r="F4" s="3">
         <v>2.1</v>
       </c>
-      <c r="F4" s="3">
+      <c r="G4" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
         <v>46</v>
       </c>
-      <c r="C5" s="3">
+      <c r="D5" s="3">
         <v>42</v>
       </c>
-      <c r="D5" s="3">
-        <v>1</v>
-      </c>
       <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3">
         <v>8</v>
       </c>
-      <c r="F5" s="3">
+      <c r="G5" s="3">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
         <v>35</v>
       </c>
-      <c r="C6" s="3">
+      <c r="D6" s="3">
         <v>8</v>
       </c>
-      <c r="D6" s="3">
+      <c r="E6" s="3">
         <v>0</v>
       </c>
-      <c r="E6" s="3">
+      <c r="F6" s="3">
         <v>3.3</v>
       </c>
-      <c r="F6" s="3">
+      <c r="G6" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3">
         <v>34</v>
       </c>
-      <c r="C7" s="3">
+      <c r="D7" s="3">
         <v>41</v>
       </c>
-      <c r="D7" s="3">
-        <v>1</v>
-      </c>
       <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
         <v>4</v>
       </c>
-      <c r="F7" s="3">
+      <c r="G7" s="3">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3">
         <v>32</v>
       </c>
-      <c r="C8" s="3">
+      <c r="D8" s="3">
         <v>21</v>
       </c>
-      <c r="D8" s="3">
+      <c r="E8" s="3">
         <v>0</v>
       </c>
-      <c r="E8" s="3">
+      <c r="F8" s="3">
         <v>5</v>
       </c>
-      <c r="F8" s="3">
+      <c r="G8" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
         <v>28</v>
       </c>
-      <c r="C9" s="3">
+      <c r="D9" s="3">
         <v>8</v>
       </c>
-      <c r="D9" s="3">
+      <c r="E9" s="3">
         <v>0</v>
       </c>
-      <c r="E9" s="3">
+      <c r="F9" s="3">
         <v>3.2</v>
       </c>
-      <c r="F9" s="3">
+      <c r="G9" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3">
         <v>43</v>
       </c>
-      <c r="C10" s="3">
+      <c r="D10" s="3">
         <v>21</v>
       </c>
-      <c r="D10" s="3">
+      <c r="E10" s="3">
         <v>0</v>
       </c>
-      <c r="E10" s="3">
+      <c r="F10" s="3">
         <v>2.8</v>
       </c>
-      <c r="F10" s="3">
+      <c r="G10" s="3">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3">
         <v>41</v>
       </c>
-      <c r="C11" s="3">
+      <c r="D11" s="3">
         <v>36</v>
       </c>
-      <c r="D11" s="3">
-        <v>1</v>
-      </c>
       <c r="E11" s="3">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3">
         <v>4.5999999999999996</v>
       </c>
-      <c r="F11" s="3">
+      <c r="G11" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3">
         <v>39</v>
       </c>
-      <c r="C12" s="3">
+      <c r="D12" s="3">
         <v>28</v>
       </c>
-      <c r="D12" s="3">
-        <v>1</v>
-      </c>
       <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3">
         <v>3.5</v>
       </c>
-      <c r="F12" s="3">
+      <c r="G12" s="3">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3">
         <v>54</v>
       </c>
-      <c r="C13" s="3">
+      <c r="D13" s="3">
         <v>57</v>
       </c>
-      <c r="D13" s="3">
-        <v>1</v>
-      </c>
       <c r="E13" s="3">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3">
         <v>2.4</v>
       </c>
-      <c r="F13" s="3">
+      <c r="G13" s="3">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3">
         <v>63</v>
       </c>
-      <c r="C14" s="3">
+      <c r="D14" s="3">
         <v>50</v>
       </c>
-      <c r="D14" s="3">
-        <v>1</v>
-      </c>
       <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3">
         <v>4.5</v>
       </c>
-      <c r="F14" s="3">
+      <c r="G14" s="3">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3">
         <v>65</v>
       </c>
-      <c r="C15" s="3">
+      <c r="D15" s="3">
         <v>18</v>
       </c>
-      <c r="D15" s="3">
-        <v>1</v>
-      </c>
       <c r="E15" s="3">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3">
         <v>1.2</v>
       </c>
-      <c r="F15" s="3">
+      <c r="G15" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3">
         <v>70</v>
       </c>
-      <c r="C16" s="3">
+      <c r="D16" s="3">
         <v>68</v>
       </c>
-      <c r="D16" s="3">
+      <c r="E16" s="3">
         <v>0</v>
       </c>
-      <c r="E16" s="3">
+      <c r="F16" s="3">
         <v>1.7</v>
       </c>
-      <c r="F16" s="3">
+      <c r="G16" s="3">
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3">
         <v>35</v>
       </c>
-      <c r="C17" s="3">
+      <c r="D17" s="3">
         <v>29</v>
       </c>
-      <c r="D17" s="3">
-        <v>1</v>
-      </c>
       <c r="E17" s="3">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F17" s="3">
+      <c r="G17" s="3">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3">
         <v>40</v>
       </c>
-      <c r="C18" s="3">
+      <c r="D18" s="3">
         <v>35</v>
       </c>
-      <c r="D18" s="3">
+      <c r="E18" s="3">
         <v>0</v>
       </c>
-      <c r="E18" s="3">
+      <c r="F18" s="3">
         <v>7.3</v>
       </c>
-      <c r="F18" s="3">
+      <c r="G18" s="3">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3">
         <v>35</v>
       </c>
-      <c r="C19" s="3">
+      <c r="D19" s="3">
         <v>12</v>
       </c>
-      <c r="D19" s="3">
-        <v>1</v>
-      </c>
       <c r="E19" s="3">
+        <v>1</v>
+      </c>
+      <c r="F19" s="3">
         <v>2.5</v>
       </c>
-      <c r="F19" s="3">
+      <c r="G19" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3">
         <v>34</v>
       </c>
-      <c r="C20" s="3">
+      <c r="D20" s="3">
         <v>14</v>
       </c>
-      <c r="D20" s="3">
-        <v>1</v>
-      </c>
       <c r="E20" s="3">
+        <v>1</v>
+      </c>
+      <c r="F20" s="3">
         <v>3.5</v>
       </c>
-      <c r="F20" s="3">
+      <c r="G20" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3">
         <v>53</v>
       </c>
-      <c r="C21" s="3">
+      <c r="D21" s="3">
         <v>18</v>
       </c>
-      <c r="D21" s="3">
-        <v>1</v>
-      </c>
       <c r="E21" s="3">
+        <v>1</v>
+      </c>
+      <c r="F21" s="3">
         <v>4.5</v>
       </c>
-      <c r="F21" s="3">
+      <c r="G21" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
+        <v>1</v>
+      </c>
+      <c r="C22" s="3">
         <v>49</v>
       </c>
-      <c r="C22" s="3">
+      <c r="D22" s="3">
         <v>26</v>
       </c>
-      <c r="D22" s="3">
+      <c r="E22" s="3">
         <v>0</v>
       </c>
-      <c r="E22" s="3">
+      <c r="F22" s="3">
         <v>5.2</v>
       </c>
-      <c r="F22" s="3">
+      <c r="G22" s="3">
         <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="I23" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" ht="21" x14ac:dyDescent="0.25">
+      <c r="C26" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C27" s="3" cm="1">
+        <f t="array" ref="C27:U31">TRANSPOSE(B4:F22)</f>
+        <v>1</v>
+      </c>
+      <c r="D27" s="3">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3">
+        <v>1</v>
+      </c>
+      <c r="F27" s="3">
+        <v>1</v>
+      </c>
+      <c r="G27" s="3">
+        <v>1</v>
+      </c>
+      <c r="H27" s="3">
+        <v>1</v>
+      </c>
+      <c r="I27" s="3">
+        <v>1</v>
+      </c>
+      <c r="J27" s="3">
+        <v>1</v>
+      </c>
+      <c r="K27" s="3">
+        <v>1</v>
+      </c>
+      <c r="L27" s="3">
+        <v>1</v>
+      </c>
+      <c r="M27" s="3">
+        <v>1</v>
+      </c>
+      <c r="N27" s="3">
+        <v>1</v>
+      </c>
+      <c r="O27" s="3">
+        <v>1</v>
+      </c>
+      <c r="P27" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>1</v>
+      </c>
+      <c r="R27" s="3">
+        <v>1</v>
+      </c>
+      <c r="S27" s="3">
+        <v>1</v>
+      </c>
+      <c r="T27" s="3">
+        <v>1</v>
+      </c>
+      <c r="U27" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C28" s="3">
+        <v>55</v>
+      </c>
+      <c r="D28" s="3">
+        <v>46</v>
+      </c>
+      <c r="E28" s="3">
+        <v>35</v>
+      </c>
+      <c r="F28" s="3">
+        <v>34</v>
+      </c>
+      <c r="G28" s="3">
+        <v>32</v>
+      </c>
+      <c r="H28" s="3">
+        <v>28</v>
+      </c>
+      <c r="I28" s="3">
+        <v>43</v>
+      </c>
+      <c r="J28" s="3">
+        <v>41</v>
+      </c>
+      <c r="K28" s="3">
+        <v>39</v>
+      </c>
+      <c r="L28" s="3">
+        <v>54</v>
+      </c>
+      <c r="M28" s="3">
+        <v>63</v>
+      </c>
+      <c r="N28" s="3">
+        <v>65</v>
+      </c>
+      <c r="O28" s="3">
+        <v>70</v>
+      </c>
+      <c r="P28" s="3">
+        <v>35</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>40</v>
+      </c>
+      <c r="R28" s="3">
+        <v>35</v>
+      </c>
+      <c r="S28" s="3">
+        <v>34</v>
+      </c>
+      <c r="T28" s="3">
+        <v>53</v>
+      </c>
+      <c r="U28" s="3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C29" s="3">
+        <v>49</v>
+      </c>
+      <c r="D29" s="3">
+        <v>42</v>
+      </c>
+      <c r="E29" s="3">
+        <v>8</v>
+      </c>
+      <c r="F29" s="3">
+        <v>41</v>
+      </c>
+      <c r="G29" s="3">
+        <v>21</v>
+      </c>
+      <c r="H29" s="3">
+        <v>8</v>
+      </c>
+      <c r="I29" s="3">
+        <v>21</v>
+      </c>
+      <c r="J29" s="3">
+        <v>36</v>
+      </c>
+      <c r="K29" s="3">
+        <v>28</v>
+      </c>
+      <c r="L29" s="3">
+        <v>57</v>
+      </c>
+      <c r="M29" s="3">
+        <v>50</v>
+      </c>
+      <c r="N29" s="3">
+        <v>18</v>
+      </c>
+      <c r="O29" s="3">
+        <v>68</v>
+      </c>
+      <c r="P29" s="3">
+        <v>29</v>
+      </c>
+      <c r="Q29" s="3">
+        <v>35</v>
+      </c>
+      <c r="R29" s="3">
+        <v>12</v>
+      </c>
+      <c r="S29" s="3">
+        <v>14</v>
+      </c>
+      <c r="T29" s="3">
+        <v>18</v>
+      </c>
+      <c r="U29" s="3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C30" s="3">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3">
+        <v>1</v>
+      </c>
+      <c r="E30" s="3">
+        <v>0</v>
+      </c>
+      <c r="F30" s="3">
+        <v>1</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0</v>
+      </c>
+      <c r="H30" s="3">
+        <v>0</v>
+      </c>
+      <c r="I30" s="3">
+        <v>0</v>
+      </c>
+      <c r="J30" s="3">
+        <v>1</v>
+      </c>
+      <c r="K30" s="3">
+        <v>1</v>
+      </c>
+      <c r="L30" s="3">
+        <v>1</v>
+      </c>
+      <c r="M30" s="3">
+        <v>1</v>
+      </c>
+      <c r="N30" s="3">
+        <v>1</v>
+      </c>
+      <c r="O30" s="3">
+        <v>0</v>
+      </c>
+      <c r="P30" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="3">
+        <v>0</v>
+      </c>
+      <c r="R30" s="3">
+        <v>1</v>
+      </c>
+      <c r="S30" s="3">
+        <v>1</v>
+      </c>
+      <c r="T30" s="3">
+        <v>1</v>
+      </c>
+      <c r="U30" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C31" s="3">
+        <v>2.1</v>
+      </c>
+      <c r="D31" s="3">
+        <v>8</v>
+      </c>
+      <c r="E31" s="3">
+        <v>3.3</v>
+      </c>
+      <c r="F31" s="3">
+        <v>4</v>
+      </c>
+      <c r="G31" s="3">
+        <v>5</v>
+      </c>
+      <c r="H31" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="I31" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="J31" s="3">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="K31" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="L31" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="M31" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="N31" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="O31" s="3">
+        <v>1.7</v>
+      </c>
+      <c r="P31" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>7.3</v>
+      </c>
+      <c r="R31" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="S31" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="T31" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="U31" s="3">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="33" spans="3:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="C33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C34" s="7" cm="1">
+        <f t="array" ref="C34:G38">MMULT(Xt,X)</f>
+        <v>19</v>
+      </c>
+      <c r="D34" s="7">
+        <v>851</v>
+      </c>
+      <c r="E34" s="7">
+        <v>581</v>
+      </c>
+      <c r="F34" s="7">
+        <v>11</v>
+      </c>
+      <c r="G34" s="7">
+        <v>71.600000000000009</v>
+      </c>
+      <c r="J34" s="3" cm="1">
+        <f t="array" ref="J34:J38">MMULT(Xt,y)</f>
+        <v>487</v>
+      </c>
+    </row>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C35" s="7">
+        <v>851</v>
+      </c>
+      <c r="D35" s="7">
+        <v>40807</v>
+      </c>
+      <c r="E35" s="7">
+        <v>28365</v>
+      </c>
+      <c r="F35" s="7">
+        <v>499</v>
+      </c>
+      <c r="G35" s="7">
+        <v>3112.5</v>
+      </c>
+      <c r="J35" s="3">
+        <v>23908</v>
+      </c>
+    </row>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C36" s="7">
+        <v>581</v>
+      </c>
+      <c r="D36" s="7">
+        <v>28365</v>
+      </c>
+      <c r="E36" s="7">
+        <v>23039</v>
+      </c>
+      <c r="F36" s="7">
+        <v>345</v>
+      </c>
+      <c r="G36" s="7">
+        <v>2198.6999999999998</v>
+      </c>
+      <c r="J36" s="3">
+        <v>19779</v>
+      </c>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C37" s="7">
+        <v>11</v>
+      </c>
+      <c r="D37" s="7">
+        <v>499</v>
+      </c>
+      <c r="E37" s="7">
+        <v>345</v>
+      </c>
+      <c r="F37" s="7">
+        <v>11</v>
+      </c>
+      <c r="G37" s="7">
+        <v>41</v>
+      </c>
+      <c r="J37" s="3">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C38" s="7">
+        <v>71.600000000000009</v>
+      </c>
+      <c r="D38" s="7">
+        <v>3112.5</v>
+      </c>
+      <c r="E38" s="7">
+        <v>2198.6999999999998</v>
+      </c>
+      <c r="F38" s="7">
+        <v>41</v>
+      </c>
+      <c r="G38" s="7">
+        <v>326.5</v>
+      </c>
+      <c r="J38" s="3">
+        <v>1805.2</v>
+      </c>
+    </row>
+    <row r="40" spans="3:12" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="C40" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J40" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+    </row>
+    <row r="41" spans="3:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="C41" s="8" cm="1">
+        <f t="array" ref="C41:G45">MINVERSE(XtX)</f>
+        <v>1.490495772948818</v>
+      </c>
+      <c r="D41" s="8">
+        <v>-2.5335345457022235E-2</v>
+      </c>
+      <c r="E41" s="8">
+        <v>5.83284356823936E-3</v>
+      </c>
+      <c r="F41" s="8">
+        <v>-0.11212471938582359</v>
+      </c>
+      <c r="G41" s="8">
+        <v>-0.11053842041905912</v>
+      </c>
+      <c r="J41" s="10" cm="1">
+        <f t="array" ref="J41:J45">MMULT(XtXInv, XtY)</f>
+        <v>4.1344383297336833</v>
+      </c>
+    </row>
+    <row r="42" spans="3:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="C42" s="8">
+        <v>-2.5335345457022228E-2</v>
+      </c>
+      <c r="D42" s="8">
+        <v>6.7628685935784173E-4</v>
+      </c>
+      <c r="E42" s="8">
+        <v>-3.0209265024854517E-4</v>
+      </c>
+      <c r="F42" s="8">
+        <v>-2.4448906781609884E-4</v>
+      </c>
+      <c r="G42" s="8">
+        <v>1.1739756412050409E-3</v>
+      </c>
+      <c r="J42" s="10">
+        <v>-9.4911601064952222E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="3:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="C43" s="8">
+        <v>5.8328435682393652E-3</v>
+      </c>
+      <c r="D43" s="8">
+        <v>-3.0209265024854528E-4</v>
+      </c>
+      <c r="E43" s="8">
+        <v>3.2524679060517303E-4</v>
+      </c>
+      <c r="F43" s="8">
+        <v>-2.4875963128901741E-4</v>
+      </c>
+      <c r="G43" s="8">
+        <v>-5.5831301441986445E-4</v>
+      </c>
+      <c r="J43" s="10">
+        <v>0.97270561805324762</v>
+      </c>
+    </row>
+    <row r="44" spans="3:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="C44" s="8">
+        <v>-0.11212471938582377</v>
+      </c>
+      <c r="D44" s="8">
+        <v>-2.444890678160919E-4</v>
+      </c>
+      <c r="E44" s="8">
+        <v>-2.4875963128901979E-4</v>
+      </c>
+      <c r="F44" s="8">
+        <v>0.21683946811429855</v>
+      </c>
+      <c r="G44" s="8">
+        <v>1.3648751615053703E-3</v>
+      </c>
+      <c r="J44" s="10">
+        <v>-1.3239181354985434</v>
+      </c>
+    </row>
+    <row r="45" spans="3:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="C45" s="8">
+        <v>-0.11053842041905913</v>
+      </c>
+      <c r="D45" s="8">
+        <v>1.173975641205042E-3</v>
+      </c>
+      <c r="E45" s="8">
+        <v>-5.5831301441986282E-4</v>
+      </c>
+      <c r="F45" s="8">
+        <v>1.3648751615053588E-3</v>
+      </c>
+      <c r="G45" s="8">
+        <v>1.9700320557234852E-2</v>
+      </c>
+      <c r="J45" s="10">
+        <v>-0.85703101057424647</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Review and study of matrices
</commit_message>
<xml_diff>
--- a/7_MATHS/2_Matrix/2_Multiple_Regression.xlsx
+++ b/7_MATHS/2_Matrix/2_Multiple_Regression.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CourseraPlus\7_MATHS\2_Matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7A963D-1839-4732-BFFE-C7F6DB650E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0FF92CC-BFE6-44E4-8FA2-2E370797DA04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Multi-reg" sheetId="1" r:id="rId1"/>
@@ -306,12 +306,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="170" formatCode="0.000"/>
-    <numFmt numFmtId="171" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -377,6 +377,32 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -430,9 +456,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -446,23 +472,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -996,22 +1031,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:U45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="M43" sqref="M43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="3.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="3.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1019,20 +1054,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:18" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="C3" s="5" t="s">
+    <row r="3" spans="2:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="D3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="10" t="s">
         <v>4</v>
       </c>
       <c r="I3" s="2" t="s">
@@ -1048,397 +1083,397 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="13">
         <v>55</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="13">
         <v>49</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="13">
         <v>0</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="13">
         <v>2.1</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="11">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" s="3">
         <v>1</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="13">
         <v>46</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="13">
         <v>42</v>
       </c>
-      <c r="E5" s="3">
-        <v>1</v>
-      </c>
-      <c r="F5" s="3">
+      <c r="E5" s="13">
+        <v>1</v>
+      </c>
+      <c r="F5" s="13">
         <v>8</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="11">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
         <v>1</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="13">
         <v>35</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="13">
         <v>8</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="13">
         <v>0</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="13">
         <v>3.3</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="11">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>1</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="13">
         <v>34</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="13">
         <v>41</v>
       </c>
-      <c r="E7" s="3">
-        <v>1</v>
-      </c>
-      <c r="F7" s="3">
+      <c r="E7" s="13">
+        <v>1</v>
+      </c>
+      <c r="F7" s="13">
         <v>4</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="11">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <v>1</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="13">
         <v>32</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="13">
         <v>21</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="13">
         <v>0</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="13">
         <v>5</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="11">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
         <v>1</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="13">
         <v>28</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="13">
         <v>8</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="13">
         <v>0</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="13">
         <v>3.2</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="11">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="13">
         <v>43</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="13">
         <v>21</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="13">
         <v>0</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="13">
         <v>2.8</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="11">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <v>1</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="13">
         <v>41</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="13">
         <v>36</v>
       </c>
-      <c r="E11" s="3">
-        <v>1</v>
-      </c>
-      <c r="F11" s="3">
+      <c r="E11" s="13">
+        <v>1</v>
+      </c>
+      <c r="F11" s="13">
         <v>4.5999999999999996</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="11">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <v>1</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="13">
         <v>39</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="13">
         <v>28</v>
       </c>
-      <c r="E12" s="3">
-        <v>1</v>
-      </c>
-      <c r="F12" s="3">
+      <c r="E12" s="13">
+        <v>1</v>
+      </c>
+      <c r="F12" s="13">
         <v>3.5</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="11">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <v>1</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="13">
         <v>54</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="13">
         <v>57</v>
       </c>
-      <c r="E13" s="3">
-        <v>1</v>
-      </c>
-      <c r="F13" s="3">
+      <c r="E13" s="13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="13">
         <v>2.4</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="11">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <v>1</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="13">
         <v>63</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="13">
         <v>50</v>
       </c>
-      <c r="E14" s="3">
-        <v>1</v>
-      </c>
-      <c r="F14" s="3">
+      <c r="E14" s="13">
+        <v>1</v>
+      </c>
+      <c r="F14" s="13">
         <v>4.5</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="11">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <v>1</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="13">
         <v>65</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="13">
         <v>18</v>
       </c>
-      <c r="E15" s="3">
-        <v>1</v>
-      </c>
-      <c r="F15" s="3">
+      <c r="E15" s="13">
+        <v>1</v>
+      </c>
+      <c r="F15" s="13">
         <v>1.2</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="11">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <v>1</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="13">
         <v>70</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="13">
         <v>68</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="13">
         <v>0</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="13">
         <v>1.7</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="11">
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <v>1</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="13">
         <v>35</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="13">
         <v>29</v>
       </c>
-      <c r="E17" s="3">
-        <v>1</v>
-      </c>
-      <c r="F17" s="3">
+      <c r="E17" s="13">
+        <v>1</v>
+      </c>
+      <c r="F17" s="13">
         <v>2.2999999999999998</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="11">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <v>1</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="13">
         <v>40</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="13">
         <v>35</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="13">
         <v>0</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="13">
         <v>7.3</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18" s="11">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <v>1</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="13">
         <v>35</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="13">
         <v>12</v>
       </c>
-      <c r="E19" s="3">
-        <v>1</v>
-      </c>
-      <c r="F19" s="3">
+      <c r="E19" s="13">
+        <v>1</v>
+      </c>
+      <c r="F19" s="13">
         <v>2.5</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="11">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <v>1</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="13">
         <v>34</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="13">
         <v>14</v>
       </c>
-      <c r="E20" s="3">
-        <v>1</v>
-      </c>
-      <c r="F20" s="3">
+      <c r="E20" s="13">
+        <v>1</v>
+      </c>
+      <c r="F20" s="13">
         <v>3.5</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="11">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <v>1</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="13">
         <v>53</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="13">
         <v>18</v>
       </c>
-      <c r="E21" s="3">
-        <v>1</v>
-      </c>
-      <c r="F21" s="3">
+      <c r="E21" s="13">
+        <v>1</v>
+      </c>
+      <c r="F21" s="13">
         <v>4.5</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="11">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <v>1</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="13">
         <v>49</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="13">
         <v>26</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="13">
         <v>0</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="13">
         <v>5.2</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G22" s="11">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="2:21" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:21" ht="16.2" x14ac:dyDescent="0.3">
       <c r="I23" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="2:21" ht="21" x14ac:dyDescent="0.25">
-      <c r="C26" s="6" t="s">
+    <row r="26" spans="2:21" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="C26" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C27" s="3" cm="1">
         <f t="array" ref="C27:U31">TRANSPOSE(B4:F22)</f>
         <v>1</v>
@@ -1498,7 +1533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C28" s="3">
         <v>55</v>
       </c>
@@ -1557,7 +1592,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C29" s="3">
         <v>49</v>
       </c>
@@ -1616,7 +1651,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C30" s="3">
         <v>0</v>
       </c>
@@ -1675,7 +1710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C31" s="3">
         <v>2.1</v>
       </c>
@@ -1734,29 +1769,29 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="33" spans="3:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="C33" s="6" t="s">
+    <row r="33" spans="3:12" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="C33" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J33" s="6" t="s">
+      <c r="J33" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C34" s="7" cm="1">
+    <row r="34" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C34" s="6" cm="1">
         <f t="array" ref="C34:G38">MMULT(Xt,X)</f>
         <v>19</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="6">
         <v>851</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E34" s="6">
         <v>581</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F34" s="6">
         <v>11</v>
       </c>
-      <c r="G34" s="7">
+      <c r="G34" s="6">
         <v>71.600000000000009</v>
       </c>
       <c r="J34" s="3" cm="1">
@@ -1764,195 +1799,195 @@
         <v>487</v>
       </c>
     </row>
-    <row r="35" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C35" s="7">
+    <row r="35" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C35" s="6">
         <v>851</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D35" s="6">
         <v>40807</v>
       </c>
-      <c r="E35" s="7">
+      <c r="E35" s="6">
         <v>28365</v>
       </c>
-      <c r="F35" s="7">
+      <c r="F35" s="6">
         <v>499</v>
       </c>
-      <c r="G35" s="7">
+      <c r="G35" s="6">
         <v>3112.5</v>
       </c>
       <c r="J35" s="3">
         <v>23908</v>
       </c>
     </row>
-    <row r="36" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C36" s="7">
+    <row r="36" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C36" s="6">
         <v>581</v>
       </c>
-      <c r="D36" s="7">
+      <c r="D36" s="6">
         <v>28365</v>
       </c>
-      <c r="E36" s="7">
+      <c r="E36" s="6">
         <v>23039</v>
       </c>
-      <c r="F36" s="7">
+      <c r="F36" s="6">
         <v>345</v>
       </c>
-      <c r="G36" s="7">
+      <c r="G36" s="6">
         <v>2198.6999999999998</v>
       </c>
       <c r="J36" s="3">
         <v>19779</v>
       </c>
     </row>
-    <row r="37" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C37" s="7">
+    <row r="37" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C37" s="6">
         <v>11</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D37" s="6">
         <v>499</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E37" s="6">
         <v>345</v>
       </c>
-      <c r="F37" s="7">
+      <c r="F37" s="6">
         <v>11</v>
       </c>
-      <c r="G37" s="7">
+      <c r="G37" s="6">
         <v>41</v>
       </c>
       <c r="J37" s="3">
         <v>284</v>
       </c>
     </row>
-    <row r="38" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C38" s="7">
+    <row r="38" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C38" s="6">
         <v>71.600000000000009</v>
       </c>
-      <c r="D38" s="7">
+      <c r="D38" s="6">
         <v>3112.5</v>
       </c>
-      <c r="E38" s="7">
+      <c r="E38" s="6">
         <v>2198.6999999999998</v>
       </c>
-      <c r="F38" s="7">
+      <c r="F38" s="6">
         <v>41</v>
       </c>
-      <c r="G38" s="7">
+      <c r="G38" s="6">
         <v>326.5</v>
       </c>
       <c r="J38" s="3">
         <v>1805.2</v>
       </c>
     </row>
-    <row r="40" spans="3:12" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="C40" s="6" t="s">
+    <row r="40" spans="3:12" ht="24" x14ac:dyDescent="0.3">
+      <c r="C40" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J40" s="9" t="s">
+      <c r="J40" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K40" s="9"/>
-      <c r="L40" s="9"/>
-    </row>
-    <row r="41" spans="3:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="C41" s="8" cm="1">
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
+    </row>
+    <row r="41" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C41" s="7" cm="1">
         <f t="array" ref="C41:G45">MINVERSE(XtX)</f>
         <v>1.490495772948818</v>
       </c>
-      <c r="D41" s="8">
+      <c r="D41" s="7">
         <v>-2.5335345457022235E-2</v>
       </c>
-      <c r="E41" s="8">
+      <c r="E41" s="7">
         <v>5.83284356823936E-3</v>
       </c>
-      <c r="F41" s="8">
+      <c r="F41" s="7">
         <v>-0.11212471938582359</v>
       </c>
-      <c r="G41" s="8">
+      <c r="G41" s="7">
         <v>-0.11053842041905912</v>
       </c>
-      <c r="J41" s="10" cm="1">
+      <c r="J41" s="9" cm="1">
         <f t="array" ref="J41:J45">MMULT(XtXInv, XtY)</f>
         <v>4.1344383297336833</v>
       </c>
     </row>
-    <row r="42" spans="3:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="C42" s="8">
+    <row r="42" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C42" s="7">
         <v>-2.5335345457022228E-2</v>
       </c>
-      <c r="D42" s="8">
+      <c r="D42" s="7">
         <v>6.7628685935784173E-4</v>
       </c>
-      <c r="E42" s="8">
+      <c r="E42" s="7">
         <v>-3.0209265024854517E-4</v>
       </c>
-      <c r="F42" s="8">
+      <c r="F42" s="7">
         <v>-2.4448906781609884E-4</v>
       </c>
-      <c r="G42" s="8">
+      <c r="G42" s="7">
         <v>1.1739756412050409E-3</v>
       </c>
-      <c r="J42" s="10">
+      <c r="J42" s="9">
         <v>-9.4911601064952222E-2</v>
       </c>
     </row>
-    <row r="43" spans="3:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="C43" s="8">
+    <row r="43" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C43" s="7">
         <v>5.8328435682393652E-3</v>
       </c>
-      <c r="D43" s="8">
+      <c r="D43" s="7">
         <v>-3.0209265024854528E-4</v>
       </c>
-      <c r="E43" s="8">
+      <c r="E43" s="7">
         <v>3.2524679060517303E-4</v>
       </c>
-      <c r="F43" s="8">
+      <c r="F43" s="7">
         <v>-2.4875963128901741E-4</v>
       </c>
-      <c r="G43" s="8">
+      <c r="G43" s="7">
         <v>-5.5831301441986445E-4</v>
       </c>
-      <c r="J43" s="10">
+      <c r="J43" s="9">
         <v>0.97270561805324762</v>
       </c>
     </row>
-    <row r="44" spans="3:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="C44" s="8">
+    <row r="44" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C44" s="7">
         <v>-0.11212471938582377</v>
       </c>
-      <c r="D44" s="8">
+      <c r="D44" s="7">
         <v>-2.444890678160919E-4</v>
       </c>
-      <c r="E44" s="8">
+      <c r="E44" s="7">
         <v>-2.4875963128901979E-4</v>
       </c>
-      <c r="F44" s="8">
+      <c r="F44" s="7">
         <v>0.21683946811429855</v>
       </c>
-      <c r="G44" s="8">
+      <c r="G44" s="7">
         <v>1.3648751615053703E-3</v>
       </c>
-      <c r="J44" s="10">
+      <c r="J44" s="9">
         <v>-1.3239181354985434</v>
       </c>
     </row>
-    <row r="45" spans="3:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="C45" s="8">
+    <row r="45" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C45" s="7">
         <v>-0.11053842041905913</v>
       </c>
-      <c r="D45" s="8">
+      <c r="D45" s="7">
         <v>1.173975641205042E-3</v>
       </c>
-      <c r="E45" s="8">
+      <c r="E45" s="7">
         <v>-5.5831301441986282E-4</v>
       </c>
-      <c r="F45" s="8">
+      <c r="F45" s="7">
         <v>1.3648751615053588E-3</v>
       </c>
-      <c r="G45" s="8">
+      <c r="G45" s="7">
         <v>1.9700320557234852E-2</v>
       </c>
-      <c r="J45" s="10">
+      <c r="J45" s="9">
         <v>-0.85703101057424647</v>
       </c>
     </row>

</xml_diff>